<commit_message>
done colision with normal enemy
</commit_message>
<xml_diff>
--- a/Castlevania/textures/resrc/enemy.xlsx
+++ b/Castlevania/textures/resrc/enemy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MINH\Projects\C++\Castlevania\Castlevania\textures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MINH\Projects\C++\Castlevania\Castlevania\textures\resrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC90F216-8FB2-4602-9EFD-084B167C503E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69621D0A-8271-4592-B707-E193589C1A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{A1BC5974-09B2-4013-A9D9-BA66001BE7DE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>chó NGỒI L</t>
+  </si>
+  <si>
+    <t>chó nhảy phải</t>
+  </si>
+  <si>
+    <t>Chó nhảy trái</t>
   </si>
 </sst>
 </file>
@@ -508,9 +514,9 @@
   <dimension ref="G1:M39"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1152,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="A19" sqref="A19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1516,7 +1522,7 @@
         <v>317</v>
       </c>
       <c r="B19" s="1">
-        <v>-1</v>
+        <v>10205</v>
       </c>
       <c r="C19" s="1">
         <v>-1</v>
@@ -1526,6 +1532,9 @@
       </c>
       <c r="E19" s="1">
         <v>-1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1533,7 +1542,7 @@
         <v>318</v>
       </c>
       <c r="B20" s="1">
-        <v>-1</v>
+        <v>10208</v>
       </c>
       <c r="C20" s="1">
         <v>-1</v>
@@ -1543,6 +1552,9 @@
       </c>
       <c r="E20" s="1">
         <v>-1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update bat and fish
</commit_message>
<xml_diff>
--- a/Castlevania/textures/resrc/enemy.xlsx
+++ b/Castlevania/textures/resrc/enemy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MINH\Projects\C++\Castlevania\Castlevania\textures\resrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69621D0A-8271-4592-B707-E193589C1A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9927553-0481-4130-8A58-BAB6DD236DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{A1BC5974-09B2-4013-A9D9-BA66001BE7DE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Chó nhảy trái</t>
+  </si>
+  <si>
+    <t>cửa scene 2.1</t>
+  </si>
+  <si>
+    <t>cửa 2</t>
   </si>
 </sst>
 </file>
@@ -514,9 +520,9 @@
   <dimension ref="G1:M39"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,43 +1106,82 @@
       <c r="G31" s="1">
         <v>10230</v>
       </c>
+      <c r="H31" s="3">
+        <v>700</v>
+      </c>
+      <c r="I31" s="3">
+        <v>130</v>
+      </c>
+      <c r="J31" s="3">
+        <v>716</v>
+      </c>
+      <c r="K31" s="3">
+        <v>195</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G32" s="1">
         <v>10231</v>
       </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="3">
+        <v>768</v>
+      </c>
+      <c r="I32" s="3">
+        <v>130</v>
+      </c>
+      <c r="J32" s="3">
+        <v>800</v>
+      </c>
+      <c r="K32" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G33" s="1">
         <v>10232</v>
       </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="3">
+        <v>800</v>
+      </c>
+      <c r="I33" s="3">
+        <v>130</v>
+      </c>
+      <c r="J33" s="3">
+        <v>900</v>
+      </c>
+      <c r="K33" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G34" s="1">
         <v>10233</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G35" s="1">
         <v>10234</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G36" s="1">
         <v>10235</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G37" s="1">
         <v>10236</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G38" s="1">
         <v>10237</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G39" s="1">
         <v>10238</v>
       </c>
@@ -1149,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F9FD9-44C1-4BF5-BBBD-9AA59D594FE1}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E20"/>
+      <selection activeCell="A22" sqref="A22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,6 +1619,43 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>320</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10230</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10231</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10232</v>
+      </c>
+      <c r="E22" s="1">
+        <v>10231</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>321</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10230</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>